<commit_message>
Change In P3 Project And Save Stored Procedure
</commit_message>
<xml_diff>
--- a/Document/1. SQL Data Process/Phase - 2 Production/Stock Report Depot wise SKU wise.xlsx
+++ b/Document/1. SQL Data Process/Phase - 2 Production/Stock Report Depot wise SKU wise.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\GIT\P3Tools\Document\Phase - 2 Production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COMPANY\P3toolsProject\Document\1. SQL Data Process\Phase - 2 Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507A7892-D238-49DA-A6FB-FF06FAECAD83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <definedName name="Slicer_Product_Name">#N/A</definedName>
     <definedName name="Slicer_Type">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -260,11 +259,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="165" formatCode="mm/yy"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="mm/yy"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -805,7 +804,7 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -868,7 +867,7 @@
     <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -922,7 +921,7 @@
     <xf numFmtId="1" fontId="6" fillId="2" borderId="13" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -931,16 +930,13 @@
     <xf numFmtId="2" fontId="6" fillId="2" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="11" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="11" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="9" applyAlignment="1">
@@ -952,6 +948,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1000,23 +999,6 @@
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1261,7 +1243,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
+      <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1297,7 +1279,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
+      <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1318,7 +1300,24 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="mm/yy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="mm/yy"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -1348,7 +1347,7 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -1462,32 +1461,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="StockDetails" displayName="StockDetails" ref="A2:O81" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" dataCellStyle="Comma">
-  <autoFilter ref="A2:O81" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="StockDetails" displayName="StockDetails" ref="A2:O81" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" dataCellStyle="Comma">
+  <autoFilter ref="A2:O81"/>
   <tableColumns count="15">
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Division" dataDxfId="14" dataCellStyle="Good"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Depot" dataDxfId="13" dataCellStyle="Good"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Product Name" dataDxfId="12" dataCellStyle="Good"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Pack" dataDxfId="11" dataCellStyle="Good"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BATCH" dataDxfId="10" dataCellStyle="Neutral"/>
-    <tableColumn id="1" xr3:uid="{0FDB3D19-89CD-435B-821B-5F9EA3FFBDFB}" name="Type" dataDxfId="0" dataCellStyle="Neutral">
+    <tableColumn id="16" name="Division" dataDxfId="14" dataCellStyle="Good"/>
+    <tableColumn id="15" name="Depot" dataDxfId="13" dataCellStyle="Good"/>
+    <tableColumn id="2" name="Product Name" dataDxfId="12" dataCellStyle="Good"/>
+    <tableColumn id="3" name="Pack" dataDxfId="11" dataCellStyle="Good"/>
+    <tableColumn id="5" name="BATCH" dataDxfId="10" dataCellStyle="Neutral"/>
+    <tableColumn id="1" name="Type" dataDxfId="9" dataCellStyle="Neutral">
       <calculatedColumnFormula>IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="MFG Date" dataDxfId="9" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EXP Date" dataDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Closing Balance" dataDxfId="7" dataCellStyle="Good"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="NRV Price" dataDxfId="6" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Stock Value" dataDxfId="5" dataCellStyle="Comma">
+    <tableColumn id="6" name="MFG Date" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="EXP Date" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="Closing Balance" dataDxfId="6" dataCellStyle="Good"/>
+    <tableColumn id="9" name="NRV Price" dataDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="11" name="Stock Value" dataDxfId="4" dataCellStyle="Comma">
       <calculatedColumnFormula>StockDetails[[#This Row],[Closing Balance]]*StockDetails[[#This Row],[NRV Price]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Days of Exp" dataDxfId="4" dataCellStyle="Comma">
+    <tableColumn id="12" name="Days of Exp" dataDxfId="3" dataCellStyle="Comma">
       <calculatedColumnFormula>StockDetails[[#This Row],[EXP Date]]-TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column1" dataDxfId="3" dataCellStyle="Neutral"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Days of from Manufacturing" dataDxfId="2" dataCellStyle="Comma">
+    <tableColumn id="10" name="Column1" dataDxfId="2" dataCellStyle="Neutral"/>
+    <tableColumn id="13" name="Days of from Manufacturing" dataDxfId="1" dataCellStyle="Comma">
       <calculatedColumnFormula>DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Weighted Days of Manufacturing" dataDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="14" name="Weighted Days of Manufacturing" dataDxfId="0" dataCellStyle="Comma">
       <calculatedColumnFormula>StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1757,43 +1756,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" style="30" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="6" max="6" width="16.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="30" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.3">
-      <c r="I1" s="31">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="I1" s="37">
         <f>SUBTOTAL(9,StockDetails[Stock Value])</f>
         <v>2577789.4299999997</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-    </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.3">
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>26</v>
       </c>
@@ -1809,7 +1808,7 @@
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="12" t="s">
@@ -1840,7 +1839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>28</v>
       </c>
@@ -1853,12 +1852,12 @@
       <c r="D3" s="24">
         <v>10</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="36" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F3" s="35" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G3" s="16">
         <v>43616</v>
@@ -1878,18 +1877,18 @@
       </c>
       <c r="L3">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>355</v>
+        <v>-516</v>
       </c>
       <c r="N3">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>340</v>
+        <v>1198</v>
       </c>
       <c r="O3">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>63580</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>224026</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>29</v>
       </c>
@@ -1902,12 +1901,12 @@
       <c r="D4" s="28">
         <v>200</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F4" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G4" s="17">
         <v>43890</v>
@@ -1927,18 +1926,18 @@
       </c>
       <c r="L4" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>266</v>
+        <v>-605</v>
       </c>
       <c r="N4" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>70</v>
+        <v>928</v>
       </c>
       <c r="O4" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>630</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>8352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>29</v>
       </c>
@@ -1951,12 +1950,12 @@
       <c r="D5" s="28">
         <v>200</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F5" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G5" s="17">
         <v>43921</v>
@@ -1976,18 +1975,18 @@
       </c>
       <c r="L5" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N5" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O5" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>107760</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
@@ -2000,12 +1999,12 @@
       <c r="D6" s="28">
         <v>100</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F6" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G6" s="17">
         <v>43708</v>
@@ -2025,18 +2024,18 @@
       </c>
       <c r="L6" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>266</v>
+        <v>-605</v>
       </c>
       <c r="N6" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>250</v>
+        <v>1108</v>
       </c>
       <c r="O6" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>49500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>219384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>28</v>
       </c>
@@ -2049,12 +2048,12 @@
       <c r="D7" s="28">
         <v>10</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <v>1924302</v>
       </c>
-      <c r="F7" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F7" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G7" s="17">
         <v>43830</v>
@@ -2074,18 +2073,18 @@
       </c>
       <c r="L7" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N7" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O7" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>8450</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>64220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>28</v>
       </c>
@@ -2098,12 +2097,12 @@
       <c r="D8" s="28">
         <v>10</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <v>1924301</v>
       </c>
-      <c r="F8" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F8" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G8" s="17">
         <v>43708</v>
@@ -2123,18 +2122,18 @@
       </c>
       <c r="L8" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>447</v>
+        <v>-424</v>
       </c>
       <c r="N8" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>250</v>
+        <v>1108</v>
       </c>
       <c r="O8" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>33500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>148472</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>28</v>
       </c>
@@ -2147,12 +2146,12 @@
       <c r="D9" s="28">
         <v>10</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <v>1924302</v>
       </c>
-      <c r="F9" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F9" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G9" s="17">
         <v>43830</v>
@@ -2172,18 +2171,18 @@
       </c>
       <c r="L9" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N9" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O9" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>1625390</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>12352964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>28</v>
       </c>
@@ -2196,12 +2195,12 @@
       <c r="D10" s="28">
         <v>10</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F10" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G10" s="17">
         <v>43616</v>
@@ -2221,18 +2220,18 @@
       </c>
       <c r="L10" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>355</v>
+        <v>-516</v>
       </c>
       <c r="N10" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>340</v>
+        <v>1198</v>
       </c>
       <c r="O10" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>67320</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>237204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>28</v>
       </c>
@@ -2245,12 +2244,12 @@
       <c r="D11" s="28">
         <v>10</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="32">
         <v>1924302</v>
       </c>
-      <c r="F11" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F11" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G11" s="17">
         <v>43830</v>
@@ -2270,18 +2269,18 @@
       </c>
       <c r="L11" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N11" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O11" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>98800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>28</v>
       </c>
@@ -2294,12 +2293,12 @@
       <c r="D12" s="28">
         <v>10</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="32">
         <v>1924302</v>
       </c>
-      <c r="F12" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F12" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G12" s="17">
         <v>43830</v>
@@ -2319,18 +2318,18 @@
       </c>
       <c r="L12" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N12" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O12" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>13780</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>104728</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>28</v>
       </c>
@@ -2343,12 +2342,12 @@
       <c r="D13" s="28">
         <v>10</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <v>1924302</v>
       </c>
-      <c r="F13" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F13" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G13" s="17">
         <v>43830</v>
@@ -2368,18 +2367,18 @@
       </c>
       <c r="L13" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N13" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O13" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>32500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>247000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>28</v>
       </c>
@@ -2392,12 +2391,12 @@
       <c r="D14" s="28">
         <v>10</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="32">
         <v>1924302</v>
       </c>
-      <c r="F14" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F14" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G14" s="17">
         <v>43830</v>
@@ -2417,18 +2416,18 @@
       </c>
       <c r="L14" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N14" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O14" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>35750</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>271700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>28</v>
       </c>
@@ -2441,12 +2440,12 @@
       <c r="D15" s="28">
         <v>10</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="32">
         <v>1924301</v>
       </c>
-      <c r="F15" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F15" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G15" s="17">
         <v>43708</v>
@@ -2466,18 +2465,18 @@
       </c>
       <c r="L15" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>447</v>
+        <v>-424</v>
       </c>
       <c r="N15" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>250</v>
+        <v>1108</v>
       </c>
       <c r="O15" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>13250</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>58724</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>28</v>
       </c>
@@ -2490,12 +2489,12 @@
       <c r="D16" s="28">
         <v>10</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="32">
         <v>1924302</v>
       </c>
-      <c r="F16" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F16" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G16" s="17">
         <v>43829</v>
@@ -2515,18 +2514,18 @@
       </c>
       <c r="L16" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>568</v>
+        <v>-303</v>
       </c>
       <c r="N16" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O16" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>7150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+        <v>54340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>28</v>
       </c>
@@ -2539,12 +2538,12 @@
       <c r="D17" s="28">
         <v>10</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="32">
         <v>1924302</v>
       </c>
-      <c r="F17" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F17" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G17" s="17">
         <v>43830</v>
@@ -2564,18 +2563,18 @@
       </c>
       <c r="L17" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N17" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O17" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>33930</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <v>257868</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>29</v>
       </c>
@@ -2588,12 +2587,12 @@
       <c r="D18" s="28">
         <v>114</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F18" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G18" s="17">
         <v>43951</v>
@@ -2613,18 +2612,18 @@
       </c>
       <c r="L18" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N18" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O18" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+        <v>143220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>29</v>
       </c>
@@ -2637,12 +2636,12 @@
       <c r="D19" s="28">
         <v>114</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F19" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G19" s="17">
         <v>43951</v>
@@ -2662,18 +2661,18 @@
       </c>
       <c r="L19" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N19" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O19" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>118048</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>29</v>
       </c>
@@ -2686,12 +2685,12 @@
       <c r="D20" s="28">
         <v>114</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F20" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G20" s="17">
         <v>43951</v>
@@ -2711,18 +2710,18 @@
       </c>
       <c r="L20" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N20" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O20" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>29</v>
       </c>
@@ -2735,12 +2734,12 @@
       <c r="D21" s="28">
         <v>114</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F21" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G21" s="17">
         <v>43951</v>
@@ -2760,18 +2759,18 @@
       </c>
       <c r="L21" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N21" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O21" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>6990</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <v>606732</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>29</v>
       </c>
@@ -2784,12 +2783,12 @@
       <c r="D22" s="28">
         <v>200</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F22" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G22" s="17">
         <v>43951</v>
@@ -2809,18 +2808,18 @@
       </c>
       <c r="L22" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N22" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O22" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>10360</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+        <v>899248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>29</v>
       </c>
@@ -2833,12 +2832,12 @@
       <c r="D23" s="28">
         <v>200</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F23" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G23" s="17">
         <v>43951</v>
@@ -2858,18 +2857,18 @@
       </c>
       <c r="L23" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N23" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O23" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13888</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>29</v>
       </c>
@@ -2882,12 +2881,12 @@
       <c r="D24" s="28">
         <v>200</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F24" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G24" s="17">
         <v>43951</v>
@@ -2907,18 +2906,18 @@
       </c>
       <c r="L24" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N24" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O24" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>20100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1744680</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>29</v>
       </c>
@@ -2931,12 +2930,12 @@
       <c r="D25" s="28">
         <v>200</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F25" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G25" s="17">
         <v>43951</v>
@@ -2956,18 +2955,18 @@
       </c>
       <c r="L25" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N25" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O25" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>24900</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2161320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>29</v>
       </c>
@@ -2980,12 +2979,12 @@
       <c r="D26" s="28">
         <v>200</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F26" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G26" s="17">
         <v>43799</v>
@@ -3005,18 +3004,18 @@
       </c>
       <c r="L26" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>174</v>
+        <v>-697</v>
       </c>
       <c r="N26" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>160</v>
+        <v>1018</v>
       </c>
       <c r="O26" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>29</v>
       </c>
@@ -3029,12 +3028,12 @@
       <c r="D27" s="28">
         <v>200</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F27" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G27" s="17">
         <v>43951</v>
@@ -3054,18 +3053,18 @@
       </c>
       <c r="L27" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N27" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O27" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>99920</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+        <v>8673056</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>29</v>
       </c>
@@ -3078,12 +3077,12 @@
       <c r="D28" s="28">
         <v>200</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="F28" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F28" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G28" s="17">
         <v>43951</v>
@@ -3103,18 +3102,18 @@
       </c>
       <c r="L28" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N28" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O28" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>370</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <v>32116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>29</v>
       </c>
@@ -3127,12 +3126,12 @@
       <c r="D29" s="28">
         <v>200</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F29" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G29" s="17">
         <v>43951</v>
@@ -3152,18 +3151,18 @@
       </c>
       <c r="L29" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N29" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O29" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>5420</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+        <v>470456</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>29</v>
       </c>
@@ -3176,12 +3175,12 @@
       <c r="D30" s="28">
         <v>200</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="E30" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F30" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G30" s="17">
         <v>43951</v>
@@ -3201,18 +3200,18 @@
       </c>
       <c r="L30" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N30" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O30" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
@@ -3225,12 +3224,12 @@
       <c r="D31" s="28">
         <v>450</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F31" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G31" s="17">
         <v>43951</v>
@@ -3250,18 +3249,18 @@
       </c>
       <c r="L31" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N31" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O31" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>13030</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1131004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>29</v>
       </c>
@@ -3274,12 +3273,12 @@
       <c r="D32" s="28">
         <v>450</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F32" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G32" s="17">
         <v>43921</v>
@@ -3299,18 +3298,18 @@
       </c>
       <c r="L32" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N32" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O32" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>8680</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+        <v>194866</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>29</v>
       </c>
@@ -3323,12 +3322,12 @@
       <c r="D33" s="28">
         <v>450</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F33" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G33" s="17">
         <v>43951</v>
@@ -3348,18 +3347,18 @@
       </c>
       <c r="L33" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N33" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O33" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+        <v>5208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>29</v>
       </c>
@@ -3372,12 +3371,12 @@
       <c r="D34" s="28">
         <v>450</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F34" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G34" s="17">
         <v>43951</v>
@@ -3397,18 +3396,18 @@
       </c>
       <c r="L34" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N34" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O34" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>29</v>
       </c>
@@ -3421,12 +3420,12 @@
       <c r="D35" s="28">
         <v>450</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F35" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G35" s="17">
         <v>43951</v>
@@ -3446,18 +3445,18 @@
       </c>
       <c r="L35" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N35" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O35" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+        <v>13020</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>29</v>
       </c>
@@ -3470,12 +3469,12 @@
       <c r="D36" s="28">
         <v>450</v>
       </c>
-      <c r="E36" s="33" t="s">
+      <c r="E36" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="F36" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F36" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G36" s="17">
         <v>43951</v>
@@ -3495,18 +3494,18 @@
       </c>
       <c r="L36" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N36" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O36" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+        <v>6076</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>29</v>
       </c>
@@ -3519,12 +3518,12 @@
       <c r="D37" s="28">
         <v>450</v>
       </c>
-      <c r="E37" s="33" t="s">
+      <c r="E37" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F37" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F37" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G37" s="17">
         <v>43799</v>
@@ -3544,18 +3543,18 @@
       </c>
       <c r="L37" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>174</v>
+        <v>-697</v>
       </c>
       <c r="N37" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>160</v>
+        <v>1018</v>
       </c>
       <c r="O37" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>29</v>
       </c>
@@ -3568,12 +3567,12 @@
       <c r="D38" s="28">
         <v>450</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="E38" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F38" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G38" s="17">
         <v>43951</v>
@@ -3593,18 +3592,18 @@
       </c>
       <c r="L38" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N38" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O38" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>570</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+        <v>49476</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>28</v>
       </c>
@@ -3617,12 +3616,12 @@
       <c r="D39" s="28">
         <v>100</v>
       </c>
-      <c r="E39" s="33" t="s">
+      <c r="E39" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F39" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G39" s="17">
         <v>43951</v>
@@ -3642,18 +3641,18 @@
       </c>
       <c r="L39" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N39" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O39" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>8650</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+        <v>750820</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>28</v>
       </c>
@@ -3666,12 +3665,12 @@
       <c r="D40" s="28">
         <v>100</v>
       </c>
-      <c r="E40" s="33" t="s">
+      <c r="E40" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="F40" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F40" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G40" s="17">
         <v>43951</v>
@@ -3691,18 +3690,18 @@
       </c>
       <c r="L40" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N40" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O40" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>38400</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3333120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>28</v>
       </c>
@@ -3715,12 +3714,12 @@
       <c r="D41" s="28">
         <v>100</v>
       </c>
-      <c r="E41" s="33" t="s">
+      <c r="E41" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F41" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G41" s="17">
         <v>43951</v>
@@ -3740,18 +3739,18 @@
       </c>
       <c r="L41" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N41" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O41" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>10570</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+        <v>917476</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>28</v>
       </c>
@@ -3764,12 +3763,12 @@
       <c r="D42" s="28">
         <v>100</v>
       </c>
-      <c r="E42" s="33" t="s">
+      <c r="E42" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F42" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G42" s="17">
         <v>43951</v>
@@ -3789,18 +3788,18 @@
       </c>
       <c r="L42" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N42" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O42" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+        <v>78120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>28</v>
       </c>
@@ -3813,12 +3812,12 @@
       <c r="D43" s="28">
         <v>100</v>
       </c>
-      <c r="E43" s="33" t="s">
+      <c r="E43" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F43" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F43" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G43" s="17">
         <v>43951</v>
@@ -3838,18 +3837,18 @@
       </c>
       <c r="L43" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N43" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O43" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>2880</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+        <v>249984</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>28</v>
       </c>
@@ -3862,12 +3861,12 @@
       <c r="D44" s="28">
         <v>100</v>
       </c>
-      <c r="E44" s="33" t="s">
+      <c r="E44" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="F44" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F44" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G44" s="17">
         <v>43951</v>
@@ -3887,18 +3886,18 @@
       </c>
       <c r="L44" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N44" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O44" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2604</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>28</v>
       </c>
@@ -3911,12 +3910,12 @@
       <c r="D45" s="28">
         <v>100</v>
       </c>
-      <c r="E45" s="33" t="s">
+      <c r="E45" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F45" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F45" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G45" s="17">
         <v>43951</v>
@@ -3936,18 +3935,18 @@
       </c>
       <c r="L45" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N45" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O45" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>3840</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+        <v>333312</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>28</v>
       </c>
@@ -3960,12 +3959,12 @@
       <c r="D46" s="28">
         <v>100</v>
       </c>
-      <c r="E46" s="33" t="s">
+      <c r="E46" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F46" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F46" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G46" s="17">
         <v>43951</v>
@@ -3985,18 +3984,18 @@
       </c>
       <c r="L46" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N46" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O46" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+        <v>166656</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>28</v>
       </c>
@@ -4009,12 +4008,12 @@
       <c r="D47" s="28">
         <v>100</v>
       </c>
-      <c r="E47" s="33" t="s">
+      <c r="E47" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F47" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G47" s="17">
         <v>43921</v>
@@ -4034,18 +4033,18 @@
       </c>
       <c r="L47" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>478</v>
+        <v>-393</v>
       </c>
       <c r="N47" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O47" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+        <v>24246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>28</v>
       </c>
@@ -4058,12 +4057,12 @@
       <c r="D48" s="28">
         <v>100</v>
       </c>
-      <c r="E48" s="33" t="s">
+      <c r="E48" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F48" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F48" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G48" s="17">
         <v>43951</v>
@@ -4083,18 +4082,18 @@
       </c>
       <c r="L48" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N48" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O48" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>9910</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+        <v>860188</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>28</v>
       </c>
@@ -4107,12 +4106,12 @@
       <c r="D49" s="28">
         <v>100</v>
       </c>
-      <c r="E49" s="33" t="s">
+      <c r="E49" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="F49" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F49" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G49" s="17">
         <v>43951</v>
@@ -4132,18 +4131,18 @@
       </c>
       <c r="L49" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N49" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O49" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+        <v>12152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>28</v>
       </c>
@@ -4156,12 +4155,12 @@
       <c r="D50" s="28">
         <v>100</v>
       </c>
-      <c r="E50" s="33" t="s">
+      <c r="E50" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F50" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F50" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G50" s="17">
         <v>43951</v>
@@ -4181,18 +4180,18 @@
       </c>
       <c r="L50" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N50" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O50" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>5180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+        <v>449624</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>28</v>
       </c>
@@ -4205,12 +4204,12 @@
       <c r="D51" s="28">
         <v>100</v>
       </c>
-      <c r="E51" s="33" t="s">
+      <c r="E51" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F51" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F51" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G51" s="17">
         <v>43951</v>
@@ -4230,18 +4229,18 @@
       </c>
       <c r="L51" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N51" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O51" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>7660</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+        <v>664888</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>29</v>
       </c>
@@ -4254,12 +4253,12 @@
       <c r="D52" s="28">
         <v>10</v>
       </c>
-      <c r="E52" s="33">
+      <c r="E52" s="32">
         <v>1924302</v>
       </c>
-      <c r="F52" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F52" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G52" s="17">
         <v>43830</v>
@@ -4279,18 +4278,18 @@
       </c>
       <c r="L52" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N52" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O52" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>4290</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+        <v>32604</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>29</v>
       </c>
@@ -4303,12 +4302,12 @@
       <c r="D53" s="28">
         <v>114</v>
       </c>
-      <c r="E53" s="33" t="s">
+      <c r="E53" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F53" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F53" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G53" s="17">
         <v>43921</v>
@@ -4328,18 +4327,18 @@
       </c>
       <c r="L53" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N53" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O53" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>8640</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+        <v>193968</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
         <v>29</v>
       </c>
@@ -4352,12 +4351,12 @@
       <c r="D54" s="28">
         <v>200</v>
       </c>
-      <c r="E54" s="33" t="s">
+      <c r="E54" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="F54" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F54" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G54" s="17">
         <v>43921</v>
@@ -4377,18 +4376,18 @@
       </c>
       <c r="L54" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N54" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O54" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>3760</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+        <v>84412</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
         <v>29</v>
       </c>
@@ -4401,12 +4400,12 @@
       <c r="D55" s="28">
         <v>450</v>
       </c>
-      <c r="E55" s="33" t="s">
+      <c r="E55" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="F55" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F55" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G55" s="17">
         <v>43921</v>
@@ -4426,18 +4425,18 @@
       </c>
       <c r="L55" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N55" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O55" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>440</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+        <v>9878</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>28</v>
       </c>
@@ -4450,12 +4449,12 @@
       <c r="D56" s="28">
         <v>10</v>
       </c>
-      <c r="E56" s="33">
+      <c r="E56" s="32">
         <v>1924301</v>
       </c>
-      <c r="F56" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F56" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G56" s="17">
         <v>43708</v>
@@ -4475,18 +4474,18 @@
       </c>
       <c r="L56" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>447</v>
+        <v>-424</v>
       </c>
       <c r="N56" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>250</v>
+        <v>1108</v>
       </c>
       <c r="O56" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>52250</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+        <v>231572</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
         <v>29</v>
       </c>
@@ -4499,12 +4498,12 @@
       <c r="D57" s="28">
         <v>200</v>
       </c>
-      <c r="E57" s="33" t="s">
+      <c r="E57" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="F57" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F57" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G57" s="17">
         <v>43951</v>
@@ -4524,18 +4523,18 @@
       </c>
       <c r="L57" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N57" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O57" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>850</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+        <v>73780</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
         <v>29</v>
       </c>
@@ -4548,12 +4547,12 @@
       <c r="D58" s="28">
         <v>450</v>
       </c>
-      <c r="E58" s="33" t="s">
+      <c r="E58" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F58" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F58" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G58" s="17">
         <v>43951</v>
@@ -4573,18 +4572,18 @@
       </c>
       <c r="L58" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N58" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O58" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>1960</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+        <v>170128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
         <v>29</v>
       </c>
@@ -4597,12 +4596,12 @@
       <c r="D59" s="28">
         <v>450</v>
       </c>
-      <c r="E59" s="33" t="s">
+      <c r="E59" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="F59" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F59" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G59" s="17">
         <v>43951</v>
@@ -4622,18 +4621,18 @@
       </c>
       <c r="L59" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N59" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O59" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>20200</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1753360</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>28</v>
       </c>
@@ -4646,12 +4645,12 @@
       <c r="D60" s="28">
         <v>100</v>
       </c>
-      <c r="E60" s="33" t="s">
+      <c r="E60" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="F60" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Dying</v>
+      <c r="F60" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G60" s="17">
         <v>43646</v>
@@ -4671,18 +4670,18 @@
       </c>
       <c r="L60" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>204</v>
+        <v>-667</v>
       </c>
       <c r="N60" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>310</v>
+        <v>1168</v>
       </c>
       <c r="O60" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>43710</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+        <v>164688</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>28</v>
       </c>
@@ -4695,12 +4694,12 @@
       <c r="D61" s="28">
         <v>100</v>
       </c>
-      <c r="E61" s="33" t="s">
+      <c r="E61" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="F61" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Dying</v>
+      <c r="F61" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G61" s="17">
         <v>43646</v>
@@ -4720,18 +4719,18 @@
       </c>
       <c r="L61" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>204</v>
+        <v>-667</v>
       </c>
       <c r="N61" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>310</v>
+        <v>1168</v>
       </c>
       <c r="O61" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>37200</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+        <v>140160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>28</v>
       </c>
@@ -4744,12 +4743,12 @@
       <c r="D62" s="28">
         <v>100</v>
       </c>
-      <c r="E62" s="33" t="s">
+      <c r="E62" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F62" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Dying</v>
+      <c r="F62" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G62" s="17">
         <v>43616</v>
@@ -4769,18 +4768,18 @@
       </c>
       <c r="L62" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>174</v>
+        <v>-697</v>
       </c>
       <c r="N62" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>340</v>
+        <v>1198</v>
       </c>
       <c r="O62" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>57460</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+        <v>202462</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>28</v>
       </c>
@@ -4793,10 +4792,10 @@
       <c r="D63" s="28">
         <v>100</v>
       </c>
-      <c r="E63" s="33" t="s">
+      <c r="E63" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F63" s="37" t="str">
+      <c r="F63" s="36" t="str">
         <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
         <v>Dead</v>
       </c>
@@ -4818,18 +4817,18 @@
       </c>
       <c r="L63" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>113</v>
+        <v>-758</v>
       </c>
       <c r="N63" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>580</v>
+        <v>1438</v>
       </c>
       <c r="O63" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>30740</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+        <v>76214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>28</v>
       </c>
@@ -4842,12 +4841,12 @@
       <c r="D64" s="28">
         <v>100</v>
       </c>
-      <c r="E64" s="33" t="s">
+      <c r="E64" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="F64" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Sick</v>
+      <c r="F64" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G64" s="17">
         <v>43738</v>
@@ -4867,18 +4866,18 @@
       </c>
       <c r="L64" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N64" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>220</v>
+        <v>1078</v>
       </c>
       <c r="O64" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>42020</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+        <v>205898</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
         <v>28</v>
       </c>
@@ -4891,12 +4890,12 @@
       <c r="D65" s="28">
         <v>10</v>
       </c>
-      <c r="E65" s="33">
+      <c r="E65" s="32">
         <v>1924302</v>
       </c>
-      <c r="F65" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F65" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G65" s="17">
         <v>43830</v>
@@ -4916,18 +4915,18 @@
       </c>
       <c r="L65" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N65" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O65" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>12480</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+        <v>94848</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
         <v>28</v>
       </c>
@@ -4940,12 +4939,12 @@
       <c r="D66" s="28">
         <v>10</v>
       </c>
-      <c r="E66" s="33">
+      <c r="E66" s="32">
         <v>1924302</v>
       </c>
-      <c r="F66" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F66" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G66" s="17">
         <v>43830</v>
@@ -4965,18 +4964,18 @@
       </c>
       <c r="L66" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N66" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O66" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>10270</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+        <v>78052</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
         <v>29</v>
       </c>
@@ -4989,12 +4988,12 @@
       <c r="D67" s="28">
         <v>114</v>
       </c>
-      <c r="E67" s="33" t="s">
+      <c r="E67" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F67" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F67" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G67" s="17">
         <v>43951</v>
@@ -5014,18 +5013,18 @@
       </c>
       <c r="L67" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N67" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O67" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+        <v>12152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
         <v>29</v>
       </c>
@@ -5038,12 +5037,12 @@
       <c r="D68" s="28">
         <v>114</v>
       </c>
-      <c r="E68" s="33" t="s">
+      <c r="E68" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F68" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F68" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G68" s="17">
         <v>43921</v>
@@ -5063,18 +5062,18 @@
       </c>
       <c r="L68" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N68" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O68" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
         <v>29</v>
       </c>
@@ -5087,12 +5086,12 @@
       <c r="D69" s="28">
         <v>200</v>
       </c>
-      <c r="E69" s="33" t="s">
+      <c r="E69" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F69" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F69" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G69" s="17">
         <v>43951</v>
@@ -5112,18 +5111,18 @@
       </c>
       <c r="L69" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N69" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O69" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>8330</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+        <v>723044</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
         <v>29</v>
       </c>
@@ -5136,12 +5135,12 @@
       <c r="D70" s="28">
         <v>200</v>
       </c>
-      <c r="E70" s="33" t="s">
+      <c r="E70" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F70" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F70" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G70" s="17">
         <v>43951</v>
@@ -5161,18 +5160,18 @@
       </c>
       <c r="L70" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N70" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O70" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>6710</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+        <v>582428</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
         <v>29</v>
       </c>
@@ -5185,12 +5184,12 @@
       <c r="D71" s="28">
         <v>450</v>
       </c>
-      <c r="E71" s="33" t="s">
+      <c r="E71" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="F71" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F71" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G71" s="17">
         <v>43951</v>
@@ -5210,18 +5209,18 @@
       </c>
       <c r="L71" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N71" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O71" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>370</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+        <v>32116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>28</v>
       </c>
@@ -5234,12 +5233,12 @@
       <c r="D72" s="28">
         <v>100</v>
       </c>
-      <c r="E72" s="33" t="s">
+      <c r="E72" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="F72" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F72" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G72" s="17">
         <v>43951</v>
@@ -5259,18 +5258,18 @@
       </c>
       <c r="L72" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N72" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O72" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>880</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+        <v>76384</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
         <v>28</v>
       </c>
@@ -5283,12 +5282,12 @@
       <c r="D73" s="28">
         <v>100</v>
       </c>
-      <c r="E73" s="33" t="s">
+      <c r="E73" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F73" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F73" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G73" s="17">
         <v>43951</v>
@@ -5308,18 +5307,18 @@
       </c>
       <c r="L73" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N73" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O73" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+        <v>166656</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>28</v>
       </c>
@@ -5332,12 +5331,12 @@
       <c r="D74" s="28">
         <v>100</v>
       </c>
-      <c r="E74" s="33" t="s">
+      <c r="E74" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="F74" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F74" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G74" s="17">
         <v>43951</v>
@@ -5357,18 +5356,18 @@
       </c>
       <c r="L74" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>508</v>
+        <v>-363</v>
       </c>
       <c r="N74" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O74" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+        <v>156240</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>28</v>
       </c>
@@ -5381,12 +5380,12 @@
       <c r="D75" s="28">
         <v>100</v>
       </c>
-      <c r="E75" s="33" t="s">
+      <c r="E75" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F75" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F75" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G75" s="17">
         <v>43890</v>
@@ -5406,18 +5405,18 @@
       </c>
       <c r="L75" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>447</v>
+        <v>-424</v>
       </c>
       <c r="N75" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>70</v>
+        <v>928</v>
       </c>
       <c r="O75" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>630</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+        <v>8352</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
         <v>34</v>
       </c>
@@ -5430,12 +5429,12 @@
       <c r="D76" s="28">
         <v>10</v>
       </c>
-      <c r="E76" s="33">
+      <c r="E76" s="32">
         <v>1924302</v>
       </c>
-      <c r="F76" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Aged</v>
+      <c r="F76" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G76" s="17">
         <v>43830</v>
@@ -5455,18 +5454,18 @@
       </c>
       <c r="L76" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>569</v>
+        <v>-302</v>
       </c>
       <c r="N76" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>130</v>
+        <v>988</v>
       </c>
       <c r="O76" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>98670</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+        <v>749892</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="25" t="s">
         <v>34</v>
       </c>
@@ -5479,12 +5478,12 @@
       <c r="D77" s="28">
         <v>114</v>
       </c>
-      <c r="E77" s="33" t="s">
+      <c r="E77" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F77" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F77" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G77" s="17">
         <v>43921</v>
@@ -5504,18 +5503,18 @@
       </c>
       <c r="L77" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N77" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O77" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>50560</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1135072</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="25" t="s">
         <v>34</v>
       </c>
@@ -5528,12 +5527,12 @@
       <c r="D78" s="28">
         <v>114</v>
       </c>
-      <c r="E78" s="33" t="s">
+      <c r="E78" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F78" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F78" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G78" s="17">
         <v>43921</v>
@@ -5553,18 +5552,18 @@
       </c>
       <c r="L78" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N78" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O78" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>76800</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1724160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="25" t="s">
         <v>34</v>
       </c>
@@ -5577,12 +5576,12 @@
       <c r="D79" s="28">
         <v>200</v>
       </c>
-      <c r="E79" s="33" t="s">
+      <c r="E79" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F79" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F79" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G79" s="17">
         <v>43951</v>
@@ -5602,18 +5601,18 @@
       </c>
       <c r="L79" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>325</v>
+        <v>-546</v>
       </c>
       <c r="N79" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>10</v>
+        <v>868</v>
       </c>
       <c r="O79" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>16680</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1447824</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="25" t="s">
         <v>34</v>
       </c>
@@ -5626,12 +5625,12 @@
       <c r="D80" s="28">
         <v>450</v>
       </c>
-      <c r="E80" s="33" t="s">
+      <c r="E80" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F80" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F80" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G80" s="17">
         <v>43921</v>
@@ -5651,18 +5650,18 @@
       </c>
       <c r="L80" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>294</v>
+        <v>-577</v>
       </c>
       <c r="N80" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="O80" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="25" t="s">
         <v>34</v>
       </c>
@@ -5675,12 +5674,12 @@
       <c r="D81" s="28">
         <v>100</v>
       </c>
-      <c r="E81" s="33" t="s">
+      <c r="E81" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F81" s="37" t="str">
-        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
-        <v>Healthy</v>
+      <c r="F81" s="36" t="str">
+        <f ca="1">IF(ISBLANK(StockDetails[[#This Row],[EXP Date]]),"-",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=85%,"Healthy",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=65%,"Aged",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=40%,"Sick",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&gt;=25%,"Dying",IF((StockDetails[[#This Row],[Days of Exp]]/(StockDetails[[#This Row],[EXP Date]]-StockDetails[[#This Row],[MFG Date]]))&lt;=10%,"Dead","Dead"))))))</f>
+        <v>Dead</v>
       </c>
       <c r="G81" s="17">
         <v>43890</v>
@@ -5700,15 +5699,15 @@
       </c>
       <c r="L81" s="13">
         <f ca="1">StockDetails[[#This Row],[EXP Date]]-TODAY()</f>
-        <v>447</v>
+        <v>-424</v>
       </c>
       <c r="N81" s="13">
         <f ca="1">DAYS360(StockDetails[[#This Row],[MFG Date]],TODAY(),FALSE)</f>
-        <v>70</v>
+        <v>928</v>
       </c>
       <c r="O81" s="14">
         <f ca="1">StockDetails[[#This Row],[Days of from Manufacturing]]*StockDetails[[#This Row],[Closing Balance]]</f>
-        <v>840</v>
+        <v>11136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>